<commit_message>
Modified Upload file template sheets order
Let the register page first, and modified the test file, update
for authorization test.
</commit_message>
<xml_diff>
--- a/td_toolkits_v3/products/tests/test_files/chip_model_test.xlsx
+++ b/td_toolkits_v3/products/tests/test_files/chip_model_test.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="upload" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
@@ -404,6 +404,7 @@
       <color rgb="FF000000"/>
       <name val="Fira Code"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -425,6 +426,7 @@
       <color rgb="FF000000"/>
       <name val="Fira Code"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -513,11 +515,11 @@
       <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.79296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="1" width="12.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="1" width="12.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.45"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14"/>
@@ -2150,7 +2152,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2173,7 +2175,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>